<commit_message>
Implement ISLOGICAL(), ISNONTEXT(), N() & NA()
</commit_message>
<xml_diff>
--- a/tests/fixtures/information.xlsx
+++ b/tests/fixtures/information.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BC2BC26-14DA-4F09-8D74-44C312E3C88F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698BAD6C-82DC-4063-A97D-18D8CD3FBD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4815" yWindow="2805" windowWidth="12090" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41055" yWindow="6750" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>iserr</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>XYZZY</t>
+  </si>
+  <si>
+    <t>na</t>
+  </si>
+  <si>
+    <t>isnontext</t>
+  </si>
+  <si>
+    <t>islogical</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -116,10 +128,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -458,13 +471,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -478,19 +491,31 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="b">
         <f>ISBLANK(A2)</f>
         <v>1</v>
@@ -508,61 +533,89 @@
         <v>1</v>
       </c>
       <c r="F2" t="b">
+        <f>ISLOGICAL(A2)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" t="b">
         <f>ISNA(A2)</f>
         <v>0</v>
       </c>
-      <c r="G2" t="b">
+      <c r="H2" t="b">
+        <f>ISNONTEXT(A2)</f>
+        <v>1</v>
+      </c>
+      <c r="I2" t="b">
         <f>ISNUMBER(A2)</f>
         <v>0</v>
       </c>
-      <c r="H2" t="b">
+      <c r="J2" t="b">
         <f>ISODD(A2)</f>
         <v>0</v>
       </c>
-      <c r="I2" t="b">
+      <c r="K2" t="b">
         <f>ISTEXT(A2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L2">
+        <f>N(A2)</f>
+        <v>0</v>
+      </c>
+      <c r="M2" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B3" t="b">
-        <f t="shared" ref="B3:B20" si="0">ISBLANK(A3)</f>
+        <f t="shared" ref="B3:B21" si="0">ISBLANK(A3)</f>
         <v>0</v>
       </c>
       <c r="C3" t="b">
-        <f t="shared" ref="C3:C20" si="1">ISERR(A3)</f>
+        <f t="shared" ref="C3:C21" si="1">ISERR(A3)</f>
         <v>1</v>
       </c>
       <c r="D3" t="b">
-        <f t="shared" ref="D3:D20" si="2">ISERROR(A3)</f>
+        <f t="shared" ref="D3:D21" si="2">ISERROR(A3)</f>
         <v>1</v>
       </c>
       <c r="E3" t="e">
-        <f t="shared" ref="E3:E20" si="3">ISEVEN(A3)</f>
+        <f t="shared" ref="E3:E21" si="3">ISEVEN(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F3" t="b">
-        <f t="shared" ref="F3:F20" si="4">ISNA(A3)</f>
+        <f t="shared" ref="F3:F21" si="4">ISLOGICAL(A3)</f>
         <v>0</v>
       </c>
       <c r="G3" t="b">
-        <f t="shared" ref="G3:G20" si="5">ISNUMBER(A3)</f>
-        <v>0</v>
-      </c>
-      <c r="H3" t="e">
-        <f t="shared" ref="H3:H20" si="6">ISODD(A3)</f>
+        <f t="shared" ref="G3:G21" si="5">ISNA(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="H3" t="b">
+        <f t="shared" ref="H3:H21" si="6">ISNONTEXT(A3)</f>
+        <v>1</v>
+      </c>
+      <c r="I3" t="b">
+        <f t="shared" ref="I3:I21" si="7">ISNUMBER(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="J3" t="e">
+        <f t="shared" ref="J3:J21" si="8">ISODD(A3)</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I3" t="b">
-        <f t="shared" ref="I3:I20" si="7">ISTEXT(A3)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="K3" t="b">
+        <f t="shared" ref="K3:K21" si="9">ISTEXT(A3)</f>
+        <v>0</v>
+      </c>
+      <c r="L3" t="e">
+        <f t="shared" ref="L3:L21" si="10">N(A3)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="e">
         <v>#NUM!</v>
       </c>
@@ -590,16 +643,28 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H4" t="e">
+      <c r="H4" t="b">
         <f t="shared" si="6"/>
-        <v>#NUM!</v>
+        <v>1</v>
       </c>
       <c r="I4" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="e">
+        <f t="shared" si="8"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L4" t="e">
+        <f t="shared" si="10"/>
+        <v>#NUM!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="e" cm="1">
         <f t="array" ref="A5">na</f>
         <v>#NAME?</v>
@@ -621,23 +686,35 @@
         <v>#NAME?</v>
       </c>
       <c r="F5" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G5" t="b">
         <f>ISNA(A5)</f>
         <v>0</v>
       </c>
-      <c r="G5" t="b">
+      <c r="H5" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
         <f>ISNUMBER(A5)</f>
         <v>0</v>
       </c>
-      <c r="H5" t="e">
+      <c r="J5" t="e">
         <f>ISODD(A5)</f>
         <v>#NAME?</v>
       </c>
-      <c r="I5" t="b">
+      <c r="K5" t="b">
         <f>ISTEXT(A5)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L5" t="e">
+        <f t="shared" si="10"/>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="e">
         <v>#VALUE!</v>
       </c>
@@ -658,23 +735,35 @@
         <v>#VALUE!</v>
       </c>
       <c r="F6" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G6" t="b">
         <f>ISNA(A6)</f>
         <v>0</v>
       </c>
-      <c r="G6" t="b">
+      <c r="H6" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
         <f>ISNUMBER(A6)</f>
         <v>0</v>
       </c>
-      <c r="H6" t="e">
+      <c r="J6" t="e">
         <f>ISODD(A6)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I6" t="b">
+      <c r="K6" t="b">
         <f>ISTEXT(A6)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L6" t="e">
+        <f t="shared" si="10"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="e">
         <v>#REF!</v>
       </c>
@@ -695,23 +784,35 @@
         <v>#REF!</v>
       </c>
       <c r="F7" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
         <f>ISNA(A7)</f>
         <v>0</v>
       </c>
-      <c r="G7" t="b">
+      <c r="H7" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I7" t="b">
         <f>ISNUMBER(A7)</f>
         <v>0</v>
       </c>
-      <c r="H7" t="e">
+      <c r="J7" t="e">
         <f>ISODD(A7)</f>
         <v>#REF!</v>
       </c>
-      <c r="I7" t="b">
+      <c r="K7" t="b">
         <f>ISTEXT(A7)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L7" t="e">
+        <f t="shared" si="10"/>
+        <v>#REF!</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="e">
         <v>#NULL!</v>
       </c>
@@ -732,24 +833,37 @@
         <v>#NULL!</v>
       </c>
       <c r="F8" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
         <f>ISNA(A8)</f>
         <v>0</v>
       </c>
-      <c r="G8" t="b">
+      <c r="H8" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I8" t="b">
         <f>ISNUMBER(A8)</f>
         <v>0</v>
       </c>
-      <c r="H8" t="e">
+      <c r="J8" t="e">
         <f>ISODD(A8)</f>
         <v>#NULL!</v>
       </c>
-      <c r="I8" t="b">
+      <c r="K8" t="b">
         <f>ISTEXT(A8)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L8" t="e">
+        <f t="shared" si="10"/>
+        <v>#NULL!</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="e">
+        <f>NA()</f>
         <v>#N/A</v>
       </c>
       <c r="B9" t="b">
@@ -769,23 +883,35 @@
         <v>#N/A</v>
       </c>
       <c r="F9" t="b">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G9" t="b">
         <f>ISNA(A9)</f>
         <v>1</v>
       </c>
-      <c r="G9" t="b">
+      <c r="H9" t="b">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="I9" t="b">
         <f>ISNUMBER(A9)</f>
         <v>0</v>
       </c>
-      <c r="H9" t="e">
+      <c r="J9" t="e">
         <f>ISODD(A9)</f>
         <v>#N/A</v>
       </c>
-      <c r="I9" t="b">
+      <c r="K9" t="b">
         <f>ISTEXT(A9)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L9" t="e">
+        <f t="shared" si="10"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -811,7 +937,7 @@
       </c>
       <c r="G10" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H10" t="b">
         <f t="shared" si="6"/>
@@ -819,10 +945,22 @@
       </c>
       <c r="I10" t="b">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J10" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="10"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0</v>
       </c>
@@ -848,18 +986,30 @@
       </c>
       <c r="G11" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H11" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I11" t="b">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -885,7 +1035,7 @@
       </c>
       <c r="G12" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12" t="b">
         <f t="shared" si="6"/>
@@ -893,10 +1043,22 @@
       </c>
       <c r="I12" t="b">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K12" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -922,18 +1084,30 @@
       </c>
       <c r="G13" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H13" t="b">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="b">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J13" t="b">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="10"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -963,14 +1137,26 @@
       </c>
       <c r="H14" t="b">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I14" t="b">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1000,14 +1186,26 @@
       </c>
       <c r="H15" t="b">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I15" t="b">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K15" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1035,16 +1233,28 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H16" t="e">
+      <c r="H16" t="b">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>0</v>
       </c>
       <c r="I16" t="b">
         <f t="shared" si="7"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="J16" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K16" t="b">
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -1066,22 +1276,34 @@
       </c>
       <c r="F17" t="b">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H17" t="e">
+      <c r="H17" t="b">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="I17" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K17" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="10"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -1103,22 +1325,34 @@
       </c>
       <c r="F18" t="b">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" t="b">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="H18" t="e">
+      <c r="H18" t="b">
         <f t="shared" si="6"/>
-        <v>#VALUE!</v>
+        <v>1</v>
       </c>
       <c r="I18" t="b">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" t="e">
+        <f t="shared" si="8"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="K18" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.23</v>
       </c>
@@ -1144,7 +1378,7 @@
       </c>
       <c r="G19" t="b">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H19" t="b">
         <f t="shared" si="6"/>
@@ -1152,44 +1386,117 @@
       </c>
       <c r="I19" t="b">
         <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="J19" t="b">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="10"/>
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>-2.34</v>
       </c>
       <c r="B20" t="b">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B20:B21" si="11">ISBLANK(A20)</f>
         <v>0</v>
       </c>
       <c r="C20" t="b">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C20:C21" si="12">ISERR(A20)</f>
         <v>0</v>
       </c>
       <c r="D20" t="b">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D20:D21" si="13">ISERROR(A20)</f>
         <v>0</v>
       </c>
       <c r="E20" t="b">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="E20:E21" si="14">ISEVEN(A20)</f>
         <v>1</v>
       </c>
       <c r="F20" t="b">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F20:F21" si="15">ISLOGICAL(A20)</f>
         <v>0</v>
       </c>
       <c r="G20" t="b">
-        <f t="shared" si="5"/>
-        <v>1</v>
+        <f t="shared" ref="G20:G21" si="16">ISNA(A20)</f>
+        <v>0</v>
       </c>
       <c r="H20" t="b">
-        <f t="shared" si="6"/>
-        <v>0</v>
+        <f t="shared" ref="H20:H21" si="17">ISNONTEXT(A20)</f>
+        <v>1</v>
       </c>
       <c r="I20" t="b">
-        <f t="shared" si="7"/>
-        <v>0</v>
+        <f t="shared" ref="I20:I21" si="18">ISNUMBER(A20)</f>
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <f t="shared" ref="J20:J21" si="19">ISODD(A20)</f>
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <f t="shared" ref="K20:K21" si="20">ISTEXT(A20)</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ref="L20:L21" si="21">N(A20)</f>
+        <v>-2.34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>36526</v>
+      </c>
+      <c r="B21" t="b">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="C21" t="b">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="D21" t="b">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="E21" t="b">
+        <f t="shared" si="14"/>
+        <v>1</v>
+      </c>
+      <c r="F21" t="b">
+        <f t="shared" si="15"/>
+        <v>0</v>
+      </c>
+      <c r="G21" t="b">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="H21" t="b">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+      <c r="I21" t="b">
+        <f t="shared" si="18"/>
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="21"/>
+        <v>36526</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add support for 'CELL('contents',[reference])' command.
</commit_message>
<xml_diff>
--- a/tests/fixtures/information.xlsx
+++ b/tests/fixtures/information.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23801"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698BAD6C-82DC-4063-A97D-18D8CD3FBD1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{625E6904-1337-4788-B1F2-B4DF02987787}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41055" yWindow="6750" windowWidth="18510" windowHeight="19665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="1" r:id="rId1"/>
@@ -471,13 +471,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -515,7 +517,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" t="b">
         <f>ISBLANK(A2)</f>
         <v>1</v>
@@ -565,57 +567,57 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="e">
         <f>1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="B3" t="b">
-        <f t="shared" ref="B3:B21" si="0">ISBLANK(A3)</f>
+        <f t="shared" ref="B3:B19" si="0">ISBLANK(A3)</f>
         <v>0</v>
       </c>
       <c r="C3" t="b">
-        <f t="shared" ref="C3:C21" si="1">ISERR(A3)</f>
+        <f t="shared" ref="C3:C19" si="1">ISERR(A3)</f>
         <v>1</v>
       </c>
       <c r="D3" t="b">
-        <f t="shared" ref="D3:D21" si="2">ISERROR(A3)</f>
+        <f t="shared" ref="D3:D19" si="2">ISERROR(A3)</f>
         <v>1</v>
       </c>
       <c r="E3" t="e">
-        <f t="shared" ref="E3:E21" si="3">ISEVEN(A3)</f>
+        <f t="shared" ref="E3:E19" si="3">ISEVEN(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="F3" t="b">
-        <f t="shared" ref="F3:F21" si="4">ISLOGICAL(A3)</f>
+        <f t="shared" ref="F3:F19" si="4">ISLOGICAL(A3)</f>
         <v>0</v>
       </c>
       <c r="G3" t="b">
-        <f t="shared" ref="G3:G21" si="5">ISNA(A3)</f>
+        <f t="shared" ref="G3:G19" si="5">ISNA(A3)</f>
         <v>0</v>
       </c>
       <c r="H3" t="b">
-        <f t="shared" ref="H3:H21" si="6">ISNONTEXT(A3)</f>
+        <f t="shared" ref="H3:H19" si="6">ISNONTEXT(A3)</f>
         <v>1</v>
       </c>
       <c r="I3" t="b">
-        <f t="shared" ref="I3:I21" si="7">ISNUMBER(A3)</f>
+        <f t="shared" ref="I3:I19" si="7">ISNUMBER(A3)</f>
         <v>0</v>
       </c>
       <c r="J3" t="e">
-        <f t="shared" ref="J3:J21" si="8">ISODD(A3)</f>
+        <f t="shared" ref="J3:J19" si="8">ISODD(A3)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="K3" t="b">
-        <f t="shared" ref="K3:K21" si="9">ISTEXT(A3)</f>
+        <f t="shared" ref="K3:K19" si="9">ISTEXT(A3)</f>
         <v>0</v>
       </c>
       <c r="L3" t="e">
-        <f t="shared" ref="L3:L21" si="10">N(A3)</f>
+        <f t="shared" ref="L3:L19" si="10">N(A3)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="e">
         <v>#NUM!</v>
       </c>
@@ -664,7 +666,7 @@
         <v>#NUM!</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="e" cm="1">
         <f t="array" ref="A5">na</f>
         <v>#NAME?</v>
@@ -714,7 +716,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="e">
         <v>#VALUE!</v>
       </c>
@@ -763,7 +765,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="e">
         <v>#REF!</v>
       </c>
@@ -812,7 +814,7 @@
         <v>#REF!</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="e">
         <v>#NULL!</v>
       </c>
@@ -861,7 +863,7 @@
         <v>#NULL!</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="e">
         <f>NA()</f>
         <v>#N/A</v>
@@ -911,7 +913,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>-1</v>
       </c>
@@ -960,7 +962,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>0</v>
       </c>
@@ -1009,7 +1011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1058,7 +1060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1107,7 +1109,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>8</v>
       </c>
@@ -1156,7 +1158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>9</v>
       </c>
@@ -1205,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -1254,7 +1256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="b">
         <v>1</v>
       </c>
@@ -1303,7 +1305,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="b">
         <v>0</v>
       </c>
@@ -1352,7 +1354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>1.23</v>
       </c>
@@ -1401,7 +1403,7 @@
         <v>1.23</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>-2.34</v>
       </c>
@@ -1450,7 +1452,7 @@
         <v>-2.34</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>36526</v>
       </c>
@@ -1497,6 +1499,48 @@
       <c r="L21">
         <f t="shared" si="21"/>
         <v>36526</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B22" t="b" cm="1">
+        <f t="array" aca="1" ref="B22" ca="1">CELL("contents", B2)</f>
+        <v>1</v>
+      </c>
+      <c r="C22" t="b" cm="1">
+        <f t="array" aca="1" ref="C22" ca="1">CELL("contents", C2)</f>
+        <v>0</v>
+      </c>
+      <c r="D22" t="b" cm="1">
+        <f t="array" aca="1" ref="D22" ca="1">CELL("contents", D2)</f>
+        <v>0</v>
+      </c>
+      <c r="E22" t="b" cm="1">
+        <f t="array" aca="1" ref="E22" ca="1">CELL("contents", E2)</f>
+        <v>1</v>
+      </c>
+      <c r="F22" t="b" cm="1">
+        <f t="array" aca="1" ref="F22" ca="1">CELL("contents", F2)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" t="b" cm="1">
+        <f t="array" aca="1" ref="G22" ca="1">CELL("contents", G2)</f>
+        <v>0</v>
+      </c>
+      <c r="H22" t="b" cm="1">
+        <f t="array" aca="1" ref="H22" ca="1">CELL("contents", H2)</f>
+        <v>1</v>
+      </c>
+      <c r="I22" t="b" cm="1">
+        <f t="array" aca="1" ref="I22" ca="1">CELL("contents", I2)</f>
+        <v>0</v>
+      </c>
+      <c r="J22" t="b" cm="1">
+        <f t="array" aca="1" ref="J22" ca="1">CELL("contents", J2)</f>
+        <v>0</v>
+      </c>
+      <c r="K22" t="b" cm="1">
+        <f t="array" aca="1" ref="K22" ca="1">CELL("contents", K2)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>